<commit_message>
update wr.controller input Excel
</commit_message>
<xml_diff>
--- a/src/Excelform/WR.xlsx
+++ b/src/Excelform/WR.xlsx
@@ -599,7 +599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -711,42 +711,180 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -783,142 +921,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1601,8 +1604,8 @@
   </sheetPr>
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1623,117 +1626,117 @@
     </row>
     <row r="3" spans="1:13" ht="8.25" customHeight="1"/>
     <row r="4" spans="1:13" ht="19.5">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="101"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="48" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="102" t="s">
+      <c r="C6" s="64"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="103"/>
-      <c r="H6" s="102" t="s">
+      <c r="G6" s="100"/>
+      <c r="H6" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="103"/>
-      <c r="J6" s="102" t="s">
+      <c r="I6" s="100"/>
+      <c r="J6" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="103"/>
+      <c r="K6" s="100"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="48" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="49"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="127" t="s">
+      <c r="C7" s="64"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="128"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="66"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="94"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="48" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="49"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="129"/>
-      <c r="G8" s="130"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="68"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="95"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="95"/>
+      <c r="K8" s="97"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="64"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="129"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="68"/>
+      <c r="B9" s="119"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="106"/>
+      <c r="H9" s="95"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="95"/>
+      <c r="K9" s="97"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="48" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="49"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="132"/>
-      <c r="H10" s="97"/>
-      <c r="I10" s="98"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="98"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="107"/>
+      <c r="G10" s="108"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="72"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="48" t="s">
@@ -1745,27 +1748,27 @@
       <c r="E11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="125"/>
-      <c r="G11" s="126"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="71"/>
+      <c r="F11" s="101"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="66"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="71"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="66"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="4" t="s">
@@ -1793,7 +1796,7 @@
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="133"/>
       <c r="H14" s="13" t="s">
         <v>60</v>
       </c>
@@ -1810,7 +1813,7 @@
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="133"/>
       <c r="H15" s="13" t="s">
         <v>61</v>
       </c>
@@ -1828,7 +1831,7 @@
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="133"/>
       <c r="H16" s="13" t="s">
         <v>62</v>
       </c>
@@ -1909,90 +1912,90 @@
       <c r="K20" s="53"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="106" t="s">
+      <c r="A21" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="107"/>
-      <c r="C21" s="107"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="107"/>
-      <c r="J21" s="107"/>
-      <c r="K21" s="108"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="75"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="115"/>
-      <c r="B22" s="116"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="116"/>
-      <c r="E22" s="116"/>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="116"/>
-      <c r="I22" s="116"/>
-      <c r="J22" s="116"/>
-      <c r="K22" s="117"/>
+      <c r="A22" s="82"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="83"/>
+      <c r="J22" s="83"/>
+      <c r="K22" s="84"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="118"/>
-      <c r="B23" s="119"/>
-      <c r="C23" s="119"/>
-      <c r="D23" s="119"/>
-      <c r="E23" s="119"/>
-      <c r="F23" s="119"/>
-      <c r="G23" s="119"/>
-      <c r="H23" s="119"/>
-      <c r="I23" s="119"/>
-      <c r="J23" s="119"/>
-      <c r="K23" s="120"/>
+      <c r="A23" s="85"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="86"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="87"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="121"/>
-      <c r="B24" s="122"/>
-      <c r="C24" s="122"/>
-      <c r="D24" s="122"/>
-      <c r="E24" s="122"/>
-      <c r="F24" s="122"/>
-      <c r="G24" s="122"/>
-      <c r="H24" s="122"/>
-      <c r="I24" s="122"/>
-      <c r="J24" s="122"/>
-      <c r="K24" s="123"/>
+      <c r="A24" s="88"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="89"/>
+      <c r="J24" s="89"/>
+      <c r="K24" s="90"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="99" t="s">
+      <c r="A25" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="100"/>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
-      <c r="E25" s="100"/>
-      <c r="F25" s="100"/>
-      <c r="G25" s="100"/>
-      <c r="H25" s="100"/>
-      <c r="I25" s="100"/>
-      <c r="J25" s="100"/>
-      <c r="K25" s="101"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="109" t="s">
+      <c r="A26" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="110"/>
-      <c r="C26" s="110"/>
-      <c r="D26" s="110"/>
-      <c r="E26" s="110"/>
-      <c r="F26" s="110"/>
-      <c r="G26" s="111"/>
-      <c r="H26" s="124" t="s">
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="124"/>
-      <c r="J26" s="124"/>
-      <c r="K26" s="124"/>
+      <c r="I26" s="91"/>
+      <c r="J26" s="91"/>
+      <c r="K26" s="91"/>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="43" t="s">
@@ -2000,171 +2003,171 @@
       </c>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
-      <c r="D27" s="112" t="s">
+      <c r="D27" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="113"/>
-      <c r="F27" s="113"/>
-      <c r="G27" s="114"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="73"/>
-      <c r="J27" s="73"/>
-      <c r="K27" s="66"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="92"/>
+      <c r="I27" s="93"/>
+      <c r="J27" s="93"/>
+      <c r="K27" s="94"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="105"/>
-      <c r="C28" s="105"/>
-      <c r="D28" s="105"/>
-      <c r="E28" s="105"/>
-      <c r="F28" s="105"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="74"/>
-      <c r="K28" s="68"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="95"/>
+      <c r="I28" s="96"/>
+      <c r="J28" s="96"/>
+      <c r="K28" s="97"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="69" t="s">
+      <c r="C29" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="97"/>
-      <c r="I29" s="105"/>
-      <c r="J29" s="105"/>
-      <c r="K29" s="98"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="72"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="70"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="65"/>
       <c r="E30" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="72" t="s">
+      <c r="H30" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="72"/>
-      <c r="J30" s="72"/>
-      <c r="K30" s="72"/>
+      <c r="I30" s="120"/>
+      <c r="J30" s="120"/>
+      <c r="K30" s="120"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="70"/>
-      <c r="C31" s="70"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="73"/>
-      <c r="J31" s="73"/>
-      <c r="K31" s="66"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="92"/>
+      <c r="I31" s="93"/>
+      <c r="J31" s="93"/>
+      <c r="K31" s="94"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="69" t="s">
+      <c r="C32" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="74"/>
-      <c r="K32" s="68"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="95"/>
+      <c r="I32" s="96"/>
+      <c r="J32" s="96"/>
+      <c r="K32" s="97"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1">
       <c r="A33" s="17" t="s">
         <v>54</v>
       </c>
       <c r="B33" s="18"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="70"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="65"/>
       <c r="E33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="76"/>
-      <c r="J33" s="76"/>
-      <c r="K33" s="77"/>
+      <c r="H33" s="121"/>
+      <c r="I33" s="122"/>
+      <c r="J33" s="122"/>
+      <c r="K33" s="123"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickTop="1">
       <c r="A34" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B34" s="10"/>
-      <c r="C34" s="87" t="s">
+      <c r="C34" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="88"/>
+      <c r="D34" s="110"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
       <c r="G34" s="21"/>
-      <c r="H34" s="89" t="s">
+      <c r="H34" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="I34" s="90"/>
-      <c r="J34" s="90"/>
-      <c r="K34" s="91"/>
+      <c r="I34" s="112"/>
+      <c r="J34" s="112"/>
+      <c r="K34" s="113"/>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1">
       <c r="A35" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="69" t="s">
+      <c r="C35" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="71"/>
+      <c r="D35" s="66"/>
       <c r="E35" s="23"/>
       <c r="F35" s="6"/>
       <c r="G35" s="24"/>
-      <c r="H35" s="78" t="s">
+      <c r="H35" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="I35" s="79"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="80"/>
+      <c r="I35" s="125"/>
+      <c r="J35" s="125"/>
+      <c r="K35" s="126"/>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1">
       <c r="A36" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B36" s="2"/>
-      <c r="C36" s="69" t="s">
+      <c r="C36" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="71"/>
+      <c r="D36" s="66"/>
       <c r="E36" s="23"/>
       <c r="F36" s="6"/>
       <c r="G36" s="24"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="82"/>
-      <c r="K36" s="83"/>
+      <c r="H36" s="127"/>
+      <c r="I36" s="128"/>
+      <c r="J36" s="128"/>
+      <c r="K36" s="129"/>
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1">
       <c r="A37" s="25" t="s">
@@ -2176,10 +2179,10 @@
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="27"/>
-      <c r="H37" s="81"/>
-      <c r="I37" s="82"/>
-      <c r="J37" s="82"/>
-      <c r="K37" s="83"/>
+      <c r="H37" s="127"/>
+      <c r="I37" s="128"/>
+      <c r="J37" s="128"/>
+      <c r="K37" s="129"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28"/>
@@ -2189,10 +2192,10 @@
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="27"/>
-      <c r="H38" s="84"/>
-      <c r="I38" s="85"/>
-      <c r="J38" s="85"/>
-      <c r="K38" s="86"/>
+      <c r="H38" s="130"/>
+      <c r="I38" s="131"/>
+      <c r="J38" s="131"/>
+      <c r="K38" s="132"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="7"/>
@@ -2202,12 +2205,12 @@
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="69" t="s">
+      <c r="H39" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="I39" s="70"/>
-      <c r="J39" s="70"/>
-      <c r="K39" s="71"/>
+      <c r="I39" s="65"/>
+      <c r="J39" s="65"/>
+      <c r="K39" s="66"/>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="9"/>
@@ -2275,22 +2278,22 @@
       </c>
       <c r="F44" s="31"/>
       <c r="G44" s="10"/>
-      <c r="H44" s="65" t="s">
+      <c r="H44" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="I44" s="73"/>
-      <c r="J44" s="73"/>
-      <c r="K44" s="66"/>
+      <c r="I44" s="93"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="94"/>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="69" t="s">
+      <c r="C45" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="71"/>
+      <c r="D45" s="66"/>
       <c r="E45" s="47"/>
       <c r="F45" s="6"/>
       <c r="G45" s="24"/>
@@ -2319,24 +2322,24 @@
       <c r="K46" s="8"/>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="92" t="s">
+      <c r="A47" s="114" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="93"/>
-      <c r="C47" s="94"/>
-      <c r="D47" s="92" t="s">
+      <c r="B47" s="115"/>
+      <c r="C47" s="116"/>
+      <c r="D47" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="E47" s="93"/>
-      <c r="F47" s="94"/>
-      <c r="G47" s="95" t="s">
+      <c r="E47" s="115"/>
+      <c r="F47" s="116"/>
+      <c r="G47" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="H47" s="95"/>
-      <c r="I47" s="95" t="s">
+      <c r="H47" s="117"/>
+      <c r="I47" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="J47" s="95"/>
+      <c r="J47" s="117"/>
       <c r="K47" s="30" t="s">
         <v>40</v>
       </c>
@@ -2348,10 +2351,10 @@
       <c r="D48" s="35"/>
       <c r="E48" s="36"/>
       <c r="F48" s="37"/>
-      <c r="G48" s="65"/>
-      <c r="H48" s="66"/>
-      <c r="I48" s="65"/>
-      <c r="J48" s="66"/>
+      <c r="G48" s="92"/>
+      <c r="H48" s="94"/>
+      <c r="I48" s="92"/>
+      <c r="J48" s="94"/>
       <c r="K48" s="38"/>
     </row>
     <row r="49" spans="1:11">
@@ -2361,10 +2364,10 @@
       <c r="D49" s="39"/>
       <c r="E49" s="40"/>
       <c r="F49" s="41"/>
-      <c r="G49" s="67"/>
-      <c r="H49" s="68"/>
-      <c r="I49" s="67"/>
-      <c r="J49" s="68"/>
+      <c r="G49" s="95"/>
+      <c r="H49" s="97"/>
+      <c r="I49" s="95"/>
+      <c r="J49" s="97"/>
       <c r="K49" s="42"/>
     </row>
     <row r="50" spans="1:11">
@@ -2374,10 +2377,10 @@
       <c r="D50" s="43"/>
       <c r="E50" s="44"/>
       <c r="F50" s="45"/>
-      <c r="G50" s="97"/>
-      <c r="H50" s="98"/>
-      <c r="I50" s="97"/>
-      <c r="J50" s="98"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="72"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="72"/>
       <c r="K50" s="46"/>
     </row>
     <row r="51" spans="1:11">
@@ -2428,10 +2431,10 @@
       <c r="E54" s="36"/>
       <c r="F54" s="36"/>
       <c r="G54" s="36"/>
-      <c r="H54" s="96"/>
-      <c r="I54" s="96"/>
-      <c r="J54" s="96"/>
-      <c r="K54" s="96"/>
+      <c r="H54" s="98"/>
+      <c r="I54" s="98"/>
+      <c r="J54" s="98"/>
+      <c r="K54" s="98"/>
     </row>
     <row r="55" spans="1:11">
       <c r="E55" s="29"/>
@@ -2444,6 +2447,43 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H31:K33"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="H35:K38"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F7:G10"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="I4:K4"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A12:K12"/>
@@ -2460,43 +2500,6 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H54:K54"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F7:G10"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K33"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="H35:K38"/>
-    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094499" right="0.23622047244094499" top="0.15748031496063" bottom="0.15748031496063" header="0.31496062992126" footer="0.31496062992126"/>

</xml_diff>